<commit_message>
Added Tab with resources and URLs
</commit_message>
<xml_diff>
--- a/Finished Projects.xlsx
+++ b/Finished Projects.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nesto\Documents\Java Projects\Daily Practice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nesto\Documents\Java Projects\DailyChallenges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4185E4A8-7D0A-4366-8343-740C2ECEEC61}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9EE0B8-52C1-4E45-B771-4F3117E744B7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4120" yWindow="2040" windowWidth="28200" windowHeight="18090" xr2:uid="{76008818-6B5F-40F2-BB6C-84B595153911}"/>
+    <workbookView xWindow="4120" yWindow="2040" windowWidth="28200" windowHeight="18090" activeTab="1" xr2:uid="{76008818-6B5F-40F2-BB6C-84B595153911}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="List of Projects" sheetId="1" r:id="rId1"/>
+    <sheet name="Sources" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Project</t>
   </si>
@@ -61,6 +62,33 @@
   </si>
   <si>
     <t>enter a number and have the program generate the fibonacci sequence to that number or Nth number</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://github.com/JSmolins/Martyrs-Mega-List</t>
+  </si>
+  <si>
+    <t>https://github.com/karan/Projects#classic-algorithms</t>
+  </si>
+  <si>
+    <t>Karan Mega Project List</t>
+  </si>
+  <si>
+    <t>Martyr2's Mega Project List</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Bj6N0pEVC-I</t>
+  </si>
+  <si>
+    <t>Chess Stepping Off Point</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/dailyprogrammer/</t>
+  </si>
+  <si>
+    <t>Subreddit for Daily Challenges</t>
   </si>
 </sst>
 </file>
@@ -104,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -123,6 +151,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -440,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68B82FE0-A384-4CDB-80D8-159F0469CE06}">
   <dimension ref="B3:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -500,4 +531,65 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C895745E-0B39-487C-9598-8225E903404E}">
+  <dimension ref="C4:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="8.7265625" style="7"/>
+    <col min="3" max="3" width="51.26953125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="25.90625" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
complete fibonacci project & updated spreadsheet
</commit_message>
<xml_diff>
--- a/Finished Projects.xlsx
+++ b/Finished Projects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nesto\Documents\Java Projects\DailyChallenges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9EE0B8-52C1-4E45-B771-4F3117E744B7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFF55BD-1C3E-4319-9B22-D86E4A1C1652}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4120" yWindow="2040" windowWidth="28200" windowHeight="18090" activeTab="1" xr2:uid="{76008818-6B5F-40F2-BB6C-84B595153911}"/>
+    <workbookView xWindow="8850" yWindow="4520" windowWidth="23580" windowHeight="15010" xr2:uid="{76008818-6B5F-40F2-BB6C-84B595153911}"/>
   </bookViews>
   <sheets>
     <sheet name="List of Projects" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Project</t>
   </si>
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68B82FE0-A384-4CDB-80D8-159F0469CE06}">
   <dimension ref="B3:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -527,6 +527,15 @@
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D5" s="3">
+        <v>43516</v>
+      </c>
+      <c r="E5" s="3">
+        <v>43516</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -537,7 +546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C895745E-0B39-487C-9598-8225E903404E}">
   <dimension ref="C4:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
completed String reverse and updated spreadsheet
</commit_message>
<xml_diff>
--- a/Finished Projects.xlsx
+++ b/Finished Projects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nesto\Documents\Java Projects\DailyChallenges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFF55BD-1C3E-4319-9B22-D86E4A1C1652}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A2016D-A575-4F8C-91B9-7A0C65F3D59A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8850" yWindow="4520" windowWidth="23580" windowHeight="15010" xr2:uid="{76008818-6B5F-40F2-BB6C-84B595153911}"/>
+    <workbookView xWindow="13470" yWindow="3390" windowWidth="23580" windowHeight="15010" xr2:uid="{76008818-6B5F-40F2-BB6C-84B595153911}"/>
   </bookViews>
   <sheets>
     <sheet name="List of Projects" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Project</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Nth Digit of Pi</t>
   </si>
   <si>
-    <t>write a program to determine the Nth digit of PI</t>
-  </si>
-  <si>
     <t>Language</t>
   </si>
   <si>
@@ -61,9 +58,6 @@
     <t>Fibonacci Sequence</t>
   </si>
   <si>
-    <t>enter a number and have the program generate the fibonacci sequence to that number or Nth number</t>
-  </si>
-  <si>
     <t>URL</t>
   </si>
   <si>
@@ -89,13 +83,34 @@
   </si>
   <si>
     <t>Subreddit for Daily Challenges</t>
+  </si>
+  <si>
+    <t>Reverse a string</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Numbers</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>enter a string and the program reverses the string and prints it out.</t>
+  </si>
+  <si>
+    <t>enter a number and have the program generate the fibonacci sequence to that number or Nth number.</t>
+  </si>
+  <si>
+    <t>write a program to determine the Nth digit of PI.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +122,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -129,10 +152,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -140,9 +164,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -155,8 +176,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -469,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68B82FE0-A384-4CDB-80D8-159F0469CE06}">
-  <dimension ref="B3:F5"/>
+  <dimension ref="B3:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -480,61 +514,91 @@
     <col min="1" max="1" width="8.7265625" style="1"/>
     <col min="2" max="2" width="17.453125" style="1" customWidth="1"/>
     <col min="3" max="3" width="42.453125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.26953125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.81640625" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="11" style="8" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="13.6328125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="G3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="3">
+        <v>23</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="9">
         <v>43515</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="9">
         <v>43516</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="3">
+        <v>22</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="9">
         <v>43516</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="9">
         <v>43516</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>7</v>
+      <c r="G5" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="9">
+        <v>43516</v>
+      </c>
+      <c r="F6" s="9">
+        <v>43516</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -547,58 +611,61 @@
   <dimension ref="C4:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="8.7265625" style="7"/>
-    <col min="3" max="3" width="51.26953125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="25.90625" style="7" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="7"/>
+    <col min="1" max="2" width="8.7265625" style="6"/>
+    <col min="3" max="3" width="51.26953125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="25.90625" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="6"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="4" t="s">
+    <row r="4" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="7" t="s">
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C7" s="7" t="s">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{8069CC71-57EC-495A-B75F-7D75A7886CB2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
completed cc number validator and updated project sheet
</commit_message>
<xml_diff>
--- a/Finished Projects.xlsx
+++ b/Finished Projects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nesto\OneDrive\Documents\Java projects\DailyChallenges\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nesto\Documents\Java Projects\DailyChallenges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{86A2016D-A575-4F8C-91B9-7A0C65F3D59A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="41" xr10:uidLastSave="{C630DE51-03BA-486B-8548-E283FC319831}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B448C7E9-49E3-462D-90DD-036A4132CF43}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2370" yWindow="0" windowWidth="18150" windowHeight="13080" xr2:uid="{76008818-6B5F-40F2-BB6C-84B595153911}"/>
+    <workbookView xWindow="13470" yWindow="3390" windowWidth="23580" windowHeight="15010" xr2:uid="{76008818-6B5F-40F2-BB6C-84B595153911}"/>
   </bookViews>
   <sheets>
     <sheet name="List of Projects" sheetId="1" r:id="rId1"/>
@@ -518,22 +518,22 @@
   <dimension ref="B3:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.73046875" style="1"/>
-    <col min="2" max="2" width="17.46484375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="42.46484375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="17.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="42.453125" style="2" customWidth="1"/>
     <col min="4" max="4" width="11" style="7" customWidth="1"/>
-    <col min="5" max="5" width="13.265625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="13.59765625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="12.796875" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="8.73046875" style="1"/>
+    <col min="5" max="5" width="13.26953125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="13.6328125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
@@ -553,7 +553,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -573,7 +573,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
@@ -593,7 +593,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
@@ -613,7 +613,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
@@ -625,6 +625,9 @@
       </c>
       <c r="E7" s="8">
         <v>43517</v>
+      </c>
+      <c r="F7" s="8">
+        <v>43519</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>6</v>
@@ -643,15 +646,15 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="8.73046875" style="6"/>
-    <col min="3" max="3" width="51.265625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="25.9296875" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="8.73046875" style="6"/>
+    <col min="1" max="2" width="8.7265625" style="6"/>
+    <col min="3" max="3" width="51.26953125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="25.90625" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="6"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C4" s="10" t="s">
         <v>8</v>
       </c>
@@ -659,7 +662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C5" s="11" t="s">
         <v>9</v>
       </c>
@@ -667,7 +670,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C6" s="11" t="s">
         <v>10</v>
       </c>
@@ -675,7 +678,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C7" s="12" t="s">
         <v>13</v>
       </c>
@@ -683,7 +686,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C8" s="12" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
2 new projects fizzbuzz and count words
started and completed fizzbuzz and started count words from file. updated spreadsheet to match
</commit_message>
<xml_diff>
--- a/Finished Projects.xlsx
+++ b/Finished Projects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nesto\Documents\Java Projects\DailyChallenges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B448C7E9-49E3-462D-90DD-036A4132CF43}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F96824F-A9A4-4356-8155-E36620D49D54}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13470" yWindow="3390" windowWidth="23580" windowHeight="15010" xr2:uid="{76008818-6B5F-40F2-BB6C-84B595153911}"/>
+    <workbookView xWindow="14240" yWindow="5090" windowWidth="23580" windowHeight="15010" xr2:uid="{76008818-6B5F-40F2-BB6C-84B595153911}"/>
   </bookViews>
   <sheets>
     <sheet name="List of Projects" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>Project</t>
   </si>
@@ -110,13 +110,25 @@
   </si>
   <si>
     <t>given a credit card number calculates the checksum value and determines if its valid</t>
+  </si>
+  <si>
+    <t>FizzBuzz</t>
+  </si>
+  <si>
+    <t>prints the numbers from 1 to 100 for multiples of 3 writes fizz for multiples of 5 writes buzz for multiples of 3 and 5 writes fizzbuzz</t>
+  </si>
+  <si>
+    <t> Counts the number of individual words in a string. For added complexity read these strings in from a text file and generate a summary.</t>
+  </si>
+  <si>
+    <t>Count words in a string</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,6 +148,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF24292E"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -162,7 +181,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -188,9 +207,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -199,6 +215,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -515,26 +540,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68B82FE0-A384-4CDB-80D8-159F0469CE06}">
-  <dimension ref="B3:G7"/>
+  <dimension ref="B3:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="17.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.54296875" style="2" customWidth="1"/>
     <col min="3" max="3" width="42.453125" style="2" customWidth="1"/>
     <col min="4" max="4" width="11" style="7" customWidth="1"/>
-    <col min="5" max="5" width="13.26953125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="13.6328125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="13.6328125" style="8" customWidth="1"/>
     <col min="7" max="7" width="12.81640625" style="4" customWidth="1"/>
     <col min="8" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -543,10 +568,10 @@
       <c r="D3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="12" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -554,7 +579,7 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -574,7 +599,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -594,7 +619,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -614,7 +639,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -630,6 +655,43 @@
         <v>43519</v>
       </c>
       <c r="G7" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="8">
+        <v>43519</v>
+      </c>
+      <c r="F8" s="8">
+        <v>43519</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="8">
+        <v>43519</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -649,13 +711,13 @@
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="8.7265625" style="6"/>
-    <col min="3" max="3" width="51.26953125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="51.26953125" style="11" customWidth="1"/>
     <col min="4" max="4" width="25.90625" style="6" customWidth="1"/>
     <col min="5" max="16384" width="8.7265625" style="6"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -663,7 +725,7 @@
       </c>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="6" t="s">
@@ -671,7 +733,7 @@
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="6" t="s">
@@ -679,7 +741,7 @@
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
@@ -687,7 +749,7 @@
       </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="6" t="s">

</xml_diff>